<commit_message>
KULR & IBM Update
</commit_message>
<xml_diff>
--- a/IBM.xlsx
+++ b/IBM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1b1227f88c0f301e/stockmodels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53DA0FAF-B7A3-4803-82E1-EBB75772B003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="35" documentId="8_{53DA0FAF-B7A3-4803-82E1-EBB75772B003}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{17A513AC-956D-B24B-A899-F18BE05F842B}"/>
   <bookViews>
-    <workbookView xWindow="41145" yWindow="915" windowWidth="20955" windowHeight="14325" activeTab="1" xr2:uid="{EE86DB47-C13C-442E-923A-D5E06ED183BA}"/>
+    <workbookView xWindow="14460" yWindow="660" windowWidth="14180" windowHeight="17180" xr2:uid="{EE86DB47-C13C-442E-923A-D5E06ED183BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -772,13 +772,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC66B1A-BFBB-4954-8EA8-AB58FD812C0A}">
   <dimension ref="M2:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="2" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="13:15" x14ac:dyDescent="0.15">
       <c r="M2" t="s">
         <v>71</v>
       </c>
@@ -786,18 +786,18 @@
         <v>223.18</v>
       </c>
     </row>
-    <row r="3" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="13:15" x14ac:dyDescent="0.15">
       <c r="M3" t="s">
         <v>44</v>
       </c>
       <c r="N3" s="3">
         <v>924.64515200000005</v>
       </c>
-      <c r="O3" t="s">
+      <c r="O3" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="13:15" x14ac:dyDescent="0.15">
       <c r="M4" t="s">
         <v>72</v>
       </c>
@@ -805,38 +805,39 @@
         <f>N3*N2</f>
         <v>206362.30502336001</v>
       </c>
-    </row>
-    <row r="5" spans="13:15" x14ac:dyDescent="0.2">
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="13:15" x14ac:dyDescent="0.15">
       <c r="M5" t="s">
         <v>48</v>
       </c>
       <c r="N5" s="3">
-        <f>13197+17+505+5390</f>
-        <v>19109</v>
-      </c>
-      <c r="O5" t="s">
+        <f>13197+17+505</f>
+        <v>13719</v>
+      </c>
+      <c r="O5" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="13:15" x14ac:dyDescent="0.15">
       <c r="M6" t="s">
         <v>60</v>
       </c>
       <c r="N6" s="3">
-        <f>52980+1584</f>
-        <v>54564</v>
-      </c>
-      <c r="O6" t="s">
+        <f>52980+3599</f>
+        <v>56579</v>
+      </c>
+      <c r="O6" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="13:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="13:15" x14ac:dyDescent="0.15">
       <c r="M7" t="s">
         <v>73</v>
       </c>
       <c r="N7" s="3">
         <f>N4-N5+N6</f>
-        <v>241817.30502336001</v>
+        <v>249222.30502336001</v>
       </c>
     </row>
   </sheetData>
@@ -848,26 +849,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A25510E-78F1-4539-A534-8553E1E8CF6B}">
   <dimension ref="A1:AX73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="M29" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AQ8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P40" sqref="P40"/>
+      <selection pane="bottomRight" activeCell="Q35" sqref="Q35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="11" width="9.140625" style="2"/>
+    <col min="2" max="2" width="22.1640625" customWidth="1"/>
+    <col min="3" max="11" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.15">
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1027,7 +1028,7 @@
         <v>2026</v>
       </c>
     </row>
-    <row r="3" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1053,7 +1054,7 @@
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
     </row>
-    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:50" x14ac:dyDescent="0.15">
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="2"/>
@@ -1065,7 +1066,7 @@
       <c r="T4" s="2"/>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B5" s="5" t="s">
         <v>18</v>
       </c>
@@ -1085,19 +1086,23 @@
       <c r="L5" s="4">
         <v>4350</v>
       </c>
-      <c r="M5" s="4"/>
+      <c r="M5" s="4">
+        <v>4187</v>
+      </c>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4">
         <v>4575</v>
       </c>
-      <c r="Q5" s="4"/>
+      <c r="Q5" s="4">
+        <v>4600</v>
+      </c>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
       <c r="T5" s="4"/>
       <c r="U5" s="4"/>
     </row>
-    <row r="6" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B6" s="5" t="s">
         <v>19</v>
       </c>
@@ -1117,19 +1122,23 @@
       <c r="L6" s="4">
         <v>1943</v>
       </c>
-      <c r="M6" s="4"/>
+      <c r="M6" s="4">
+        <v>1759</v>
+      </c>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4">
         <v>2164</v>
       </c>
-      <c r="Q6" s="4"/>
+      <c r="Q6" s="4">
+        <v>1925</v>
+      </c>
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
     </row>
-    <row r="7" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
@@ -1149,19 +1158,23 @@
       <c r="L7" s="4">
         <v>2295</v>
       </c>
-      <c r="M7" s="4"/>
+      <c r="M7" s="4">
+        <v>2291</v>
+      </c>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4">
         <v>2360</v>
       </c>
-      <c r="Q7" s="4"/>
+      <c r="Q7" s="4">
+        <v>2327</v>
+      </c>
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
     </row>
-    <row r="8" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B8" s="3" t="s">
         <v>21</v>
       </c>
@@ -1181,19 +1194,23 @@
       <c r="L8" s="4">
         <v>1991</v>
       </c>
-      <c r="M8" s="4"/>
+      <c r="M8" s="4">
+        <v>1944</v>
+      </c>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4">
         <v>1902</v>
       </c>
-      <c r="Q8" s="4"/>
+      <c r="Q8" s="4">
+        <v>1921</v>
+      </c>
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
@@ -1213,19 +1230,23 @@
       <c r="L9" s="4">
         <v>941</v>
       </c>
-      <c r="M9" s="4"/>
+      <c r="M9" s="4">
+        <v>943</v>
+      </c>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4">
         <v>917</v>
       </c>
-      <c r="Q9" s="4"/>
+      <c r="Q9" s="4">
+        <v>905</v>
+      </c>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
     </row>
-    <row r="10" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1245,19 +1266,23 @@
       <c r="L10" s="4">
         <v>2260</v>
       </c>
-      <c r="M10" s="4"/>
+      <c r="M10" s="4">
+        <v>1943</v>
+      </c>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4">
         <v>2360</v>
       </c>
-      <c r="Q10" s="4"/>
+      <c r="Q10" s="4">
+        <v>1765</v>
+      </c>
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="4"/>
       <c r="U10" s="4"/>
     </row>
-    <row r="11" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
@@ -1277,19 +1302,23 @@
       <c r="L11" s="4">
         <v>1358</v>
       </c>
-      <c r="M11" s="4"/>
+      <c r="M11" s="4">
+        <v>1329</v>
+      </c>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4">
         <v>1285</v>
       </c>
-      <c r="Q11" s="4"/>
+      <c r="Q11" s="4">
+        <v>1277</v>
+      </c>
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
     </row>
-    <row r="12" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="3" t="s">
         <v>25</v>
       </c>
@@ -1309,19 +1338,23 @@
       <c r="L12" s="4">
         <v>185</v>
       </c>
-      <c r="M12" s="4"/>
+      <c r="M12" s="4">
+        <v>186</v>
+      </c>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4">
         <v>169</v>
       </c>
-      <c r="Q12" s="4"/>
+      <c r="Q12" s="4">
+        <v>181</v>
+      </c>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
     </row>
-    <row r="13" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B13" s="3" t="s">
         <v>26</v>
       </c>
@@ -1341,19 +1374,23 @@
       <c r="L13" s="4">
         <v>152</v>
       </c>
-      <c r="M13" s="4"/>
+      <c r="M13" s="4">
+        <v>170</v>
+      </c>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4">
         <v>38</v>
       </c>
-      <c r="Q13" s="4"/>
+      <c r="Q13" s="4">
+        <v>68</v>
+      </c>
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
     </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:50" x14ac:dyDescent="0.15">
       <c r="L14" s="2"/>
       <c r="M14" s="2"/>
       <c r="N14" s="2"/>
@@ -1365,7 +1402,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
     </row>
-    <row r="15" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B15" s="3" t="s">
         <v>27</v>
       </c>
@@ -1385,6 +1422,9 @@
       <c r="L15" s="4">
         <v>7553</v>
       </c>
+      <c r="M15" s="3">
+        <v>7541</v>
+      </c>
       <c r="P15" s="3">
         <v>7405</v>
       </c>
@@ -1401,7 +1441,7 @@
         <v>30206</v>
       </c>
     </row>
-    <row r="16" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:50" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B16" s="3" t="s">
         <v>28</v>
       </c>
@@ -1421,6 +1461,9 @@
       <c r="L16" s="4">
         <v>7739</v>
       </c>
+      <c r="M16" s="3">
+        <v>7025</v>
+      </c>
       <c r="P16" s="3">
         <v>8195</v>
       </c>
@@ -1437,7 +1480,7 @@
         <v>29673</v>
       </c>
     </row>
-    <row r="17" spans="2:46" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:46" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B17" s="3" t="s">
         <v>25</v>
       </c>
@@ -1457,6 +1500,9 @@
       <c r="L17" s="4">
         <v>183</v>
       </c>
+      <c r="M17" s="3">
+        <v>186</v>
+      </c>
       <c r="P17" s="3">
         <v>169</v>
       </c>
@@ -1473,7 +1519,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="18" spans="2:46" s="5" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:46" s="5" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B18" s="5" t="s">
         <v>29</v>
       </c>
@@ -1496,6 +1542,10 @@
         <f>SUM(L15:L17)</f>
         <v>15475</v>
       </c>
+      <c r="M18" s="5">
+        <f>SUM(M15:M17)</f>
+        <v>14752</v>
+      </c>
       <c r="P18" s="5">
         <f>SUM(P15:P17)</f>
         <v>15769</v>
@@ -1517,7 +1567,7 @@
         <v>60530</v>
       </c>
     </row>
-    <row r="19" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B19" s="3" t="s">
         <v>30</v>
       </c>
@@ -1530,6 +1580,9 @@
       <c r="L19" s="4">
         <v>5294</v>
       </c>
+      <c r="M19" s="3">
+        <v>5217</v>
+      </c>
       <c r="P19" s="3">
         <v>5126</v>
       </c>
@@ -1546,7 +1599,7 @@
         <v>21062</v>
       </c>
     </row>
-    <row r="20" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
@@ -1559,6 +1612,9 @@
       <c r="L20" s="4">
         <v>1587</v>
       </c>
+      <c r="M20" s="3">
+        <v>1419</v>
+      </c>
       <c r="P20" s="3">
         <v>1607</v>
       </c>
@@ -1575,7 +1631,7 @@
         <v>6374</v>
       </c>
     </row>
-    <row r="21" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B21" s="3" t="s">
         <v>32</v>
       </c>
@@ -1588,6 +1644,9 @@
       <c r="L21" s="4">
         <v>93</v>
       </c>
+      <c r="M21" s="3">
+        <v>94</v>
+      </c>
       <c r="P21" s="3">
         <v>86</v>
       </c>
@@ -1604,7 +1663,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="22" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B22" s="3" t="s">
         <v>33</v>
       </c>
@@ -1620,6 +1679,10 @@
         <f>SUM(L19:L21)</f>
         <v>6974</v>
       </c>
+      <c r="M22" s="4">
+        <f>SUM(M19:M21)</f>
+        <v>6730</v>
+      </c>
       <c r="P22" s="4">
         <f>SUM(P19:P21)</f>
         <v>6819</v>
@@ -1641,7 +1704,7 @@
         <v>27842</v>
       </c>
     </row>
-    <row r="23" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1657,6 +1720,10 @@
         <f>L18-L22</f>
         <v>8501</v>
       </c>
+      <c r="M23" s="4">
+        <f>M18-M22</f>
+        <v>8022</v>
+      </c>
       <c r="P23" s="4">
         <f>P18-P22</f>
         <v>8950</v>
@@ -1678,7 +1745,7 @@
         <v>32688</v>
       </c>
     </row>
-    <row r="24" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B24" s="3" t="s">
         <v>35</v>
       </c>
@@ -1691,6 +1758,9 @@
       <c r="L24" s="4">
         <v>4900</v>
       </c>
+      <c r="M24" s="3">
+        <v>4458</v>
+      </c>
       <c r="P24" s="3">
         <v>4938</v>
       </c>
@@ -1707,7 +1777,7 @@
         <v>18609</v>
       </c>
     </row>
-    <row r="25" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B25" s="3" t="s">
         <v>36</v>
       </c>
@@ -1720,6 +1790,9 @@
       <c r="L25" s="4">
         <v>1687</v>
       </c>
+      <c r="M25" s="3">
+        <v>1685</v>
+      </c>
       <c r="P25" s="3">
         <v>1840</v>
       </c>
@@ -1736,7 +1809,7 @@
         <v>6567</v>
       </c>
     </row>
-    <row r="26" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B26" s="3" t="s">
         <v>37</v>
       </c>
@@ -1752,6 +1825,10 @@
         <f>L24+L25</f>
         <v>6587</v>
       </c>
+      <c r="M26" s="4">
+        <f>M24+M25</f>
+        <v>6143</v>
+      </c>
       <c r="P26" s="4">
         <f>P24+P25</f>
         <v>6778</v>
@@ -1773,7 +1850,7 @@
         <v>25176</v>
       </c>
     </row>
-    <row r="27" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B27" s="3" t="s">
         <v>38</v>
       </c>
@@ -1789,6 +1866,10 @@
         <f>L23-L26</f>
         <v>1914</v>
       </c>
+      <c r="M27" s="4">
+        <f>M23-M26</f>
+        <v>1879</v>
+      </c>
       <c r="P27" s="4">
         <f>P23-P26</f>
         <v>2172</v>
@@ -1810,7 +1891,7 @@
         <v>7512</v>
       </c>
     </row>
-    <row r="28" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B28" s="3" t="s">
         <v>39</v>
       </c>
@@ -1826,6 +1907,10 @@
         <f>248+261-423</f>
         <v>86</v>
       </c>
+      <c r="M28">
+        <f>-190-215+412</f>
+        <v>7</v>
+      </c>
       <c r="P28">
         <f>241+233-427</f>
         <v>47</v>
@@ -1847,7 +1932,7 @@
         <v>-553</v>
       </c>
     </row>
-    <row r="29" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B29" s="3" t="s">
         <v>40</v>
       </c>
@@ -1863,6 +1948,10 @@
         <f>L27+L28</f>
         <v>2000</v>
       </c>
+      <c r="M29" s="4">
+        <f>M27+M28</f>
+        <v>1886</v>
+      </c>
       <c r="P29" s="4">
         <f>P27+P28</f>
         <v>2219</v>
@@ -1884,7 +1973,7 @@
         <v>6959</v>
       </c>
     </row>
-    <row r="30" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B30" s="3" t="s">
         <v>41</v>
       </c>
@@ -1899,6 +1988,9 @@
       <c r="L30">
         <v>419</v>
       </c>
+      <c r="M30">
+        <v>159</v>
+      </c>
       <c r="P30">
         <v>389</v>
       </c>
@@ -1915,7 +2007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B31" s="3" t="s">
         <v>42</v>
       </c>
@@ -1931,6 +2023,10 @@
         <f>+L29-L30</f>
         <v>1581</v>
       </c>
+      <c r="M31" s="3">
+        <f>+M29-M30</f>
+        <v>1727</v>
+      </c>
       <c r="P31" s="3">
         <f>+P29-P30</f>
         <v>1830</v>
@@ -1952,7 +2048,7 @@
         <v>6959</v>
       </c>
     </row>
-    <row r="32" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B32" s="3" t="s">
         <v>43</v>
       </c>
@@ -1968,6 +2064,10 @@
         <f>L31/L33</f>
         <v>1.7375535773161885</v>
       </c>
+      <c r="M32" s="7">
+        <f>M31/M33</f>
+        <v>1.8919807186678352</v>
+      </c>
       <c r="P32" s="7">
         <f>P31/P33</f>
         <v>1.9884820167336739</v>
@@ -1989,7 +2089,7 @@
         <v>7.7094023911444349</v>
       </c>
     </row>
-    <row r="33" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B33" s="3" t="s">
         <v>44</v>
       </c>
@@ -2005,6 +2105,9 @@
       <c r="L33" s="4">
         <v>909.9</v>
       </c>
+      <c r="M33" s="4">
+        <v>912.8</v>
+      </c>
       <c r="P33" s="4">
         <v>920.3</v>
       </c>
@@ -2021,7 +2124,7 @@
         <v>902.66399999999999</v>
       </c>
     </row>
-    <row r="35" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B35" s="3" t="s">
         <v>45</v>
       </c>
@@ -2033,13 +2136,17 @@
         <f>L18/H18-1</f>
         <v>#DIV/0!</v>
       </c>
+      <c r="M35" s="9" t="e">
+        <f>M18/I18-1</f>
+        <v>#DIV/0!</v>
+      </c>
       <c r="P35" s="9">
         <f>P18/L18-1</f>
         <v>1.8998384491114795E-2</v>
       </c>
-      <c r="Q35" s="9" t="e">
+      <c r="Q35" s="9">
         <f>Q18/M18-1</f>
-        <v>#DIV/0!</v>
+        <v>1.4574295010846061E-2</v>
       </c>
       <c r="AS35" s="10">
         <f>AS18/AR18-1</f>
@@ -2050,7 +2157,7 @@
         <v>5.5430594061132377E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B36" s="3" t="s">
         <v>46</v>
       </c>
@@ -2066,6 +2173,10 @@
         <f>L23/L18</f>
         <v>0.54933764135702745</v>
       </c>
+      <c r="M36" s="9">
+        <f>M23/M18</f>
+        <v>0.54379067245119306</v>
+      </c>
       <c r="P36" s="9">
         <f>P23/P18</f>
         <v>0.56756928150168051</v>
@@ -2087,7 +2198,7 @@
         <v>0.54002973732033699</v>
       </c>
     </row>
-    <row r="38" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B38" s="3" t="s">
         <v>47</v>
       </c>
@@ -2096,7 +2207,7 @@
         <v>-38732</v>
       </c>
     </row>
-    <row r="39" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B39" s="3" t="s">
         <v>48</v>
       </c>
@@ -2105,7 +2216,7 @@
         <v>17799</v>
       </c>
     </row>
-    <row r="40" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B40" s="3" t="s">
         <v>49</v>
       </c>
@@ -2114,7 +2225,7 @@
         <v>6526</v>
       </c>
     </row>
-    <row r="41" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B41" s="3" t="s">
         <v>50</v>
       </c>
@@ -2123,7 +2234,7 @@
         <v>11281</v>
       </c>
     </row>
-    <row r="42" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B42" s="3" t="s">
         <v>51</v>
       </c>
@@ -2131,7 +2242,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="43" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B43" s="3" t="s">
         <v>52</v>
       </c>
@@ -2140,7 +2251,7 @@
         <v>1817</v>
       </c>
     </row>
-    <row r="44" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B44" s="3" t="s">
         <v>53</v>
       </c>
@@ -2148,7 +2259,7 @@
         <v>2784</v>
       </c>
     </row>
-    <row r="45" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B45" s="3" t="s">
         <v>54</v>
       </c>
@@ -2156,7 +2267,7 @@
         <v>5600</v>
       </c>
     </row>
-    <row r="46" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B46" s="3" t="s">
         <v>55</v>
       </c>
@@ -2164,7 +2275,7 @@
         <v>3130</v>
       </c>
     </row>
-    <row r="47" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B47" s="3" t="s">
         <v>56</v>
       </c>
@@ -2172,7 +2283,7 @@
         <v>7630</v>
       </c>
     </row>
-    <row r="48" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B48" s="3" t="s">
         <v>57</v>
       </c>
@@ -2180,7 +2291,7 @@
         <v>6378</v>
       </c>
     </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B49" s="3" t="s">
         <v>58</v>
       </c>
@@ -2189,7 +2300,7 @@
         <v>69667</v>
       </c>
     </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B50" s="3" t="s">
         <v>59</v>
       </c>
@@ -2198,11 +2309,11 @@
         <v>133846</v>
       </c>
     </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B51" s="3"/>
       <c r="P51" s="3"/>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B52" s="3" t="s">
         <v>41</v>
       </c>
@@ -2210,7 +2321,7 @@
         <v>1691</v>
       </c>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B53" s="3" t="s">
         <v>60</v>
       </c>
@@ -2219,7 +2330,7 @@
         <v>56531</v>
       </c>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B54" s="3" t="s">
         <v>61</v>
       </c>
@@ -2227,7 +2338,7 @@
         <v>3631</v>
       </c>
     </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B55" s="3" t="s">
         <v>62</v>
       </c>
@@ -2235,7 +2346,7 @@
         <v>3125</v>
       </c>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B56" s="3" t="s">
         <v>63</v>
       </c>
@@ -2244,7 +2355,7 @@
         <v>17132</v>
       </c>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B57" s="3" t="s">
         <v>64</v>
       </c>
@@ -2253,7 +2364,7 @@
         <v>3308</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B58" s="3" t="s">
         <v>65</v>
       </c>
@@ -2261,7 +2372,7 @@
         <v>3195</v>
       </c>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B59" s="3" t="s">
         <v>56</v>
       </c>
@@ -2269,7 +2380,7 @@
         <v>10200</v>
       </c>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B60" s="3" t="s">
         <v>26</v>
       </c>
@@ -2277,7 +2388,7 @@
         <v>10932</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B61" s="3" t="s">
         <v>66</v>
       </c>
@@ -2285,7 +2396,7 @@
         <v>24103</v>
       </c>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.15">
       <c r="B62" s="3" t="s">
         <v>67</v>
       </c>
@@ -2294,7 +2405,7 @@
         <v>133848</v>
       </c>
     </row>
-    <row r="71" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B71" s="3" t="s">
         <v>68</v>
       </c>
@@ -2314,7 +2425,7 @@
         <v>10435</v>
       </c>
     </row>
-    <row r="72" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B72" s="3" t="s">
         <v>69</v>
       </c>
@@ -2334,7 +2445,7 @@
         <v>1346</v>
       </c>
     </row>
-    <row r="73" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B73" s="3" t="s">
         <v>70</v>
       </c>

</xml_diff>